<commit_message>
add nytf usat j lvgs
</commit_message>
<xml_diff>
--- a/webscript/usat/usat-marijuana.xlsx
+++ b/webscript/usat/usat-marijuana.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="14">
   <si>
     <t>comp_count</t>
   </si>
@@ -37,19 +37,25 @@
     <t>start_date</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>USA Today - All sources</t>
   </si>
   <si>
-    <t>19990930</t>
+    <t>ＣＢＳ</t>
+  </si>
+  <si>
+    <t>The ArcView Group</t>
+  </si>
+  <si>
+    <t>JetBlue Airways Corp.</t>
+  </si>
+  <si>
+    <t>Sears Holdings Corp</t>
+  </si>
+  <si>
+    <t>United States Customs and Border Protection</t>
   </si>
   <si>
     <t>sc=usat and la=en and ((marijuana sector) or (marijuana industry) or (marijuana-sector) or (marijuana-industry) or (medical pot sector) or (medical pot industry) or (medical pot-sector) or (medical pot-industry) or (pot sector) or (pot industry) or (pot-sector) or (pot-industry))</t>
-  </si>
-  <si>
-    <t>19990701</t>
   </si>
 </sst>
 </file>
@@ -407,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,7 +447,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>19881231</v>
@@ -453,7 +459,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>19881001</v>
@@ -464,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>19890630</v>
@@ -476,7 +482,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G3">
         <v>19890401</v>
@@ -487,7 +493,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>19900930</v>
@@ -499,7 +505,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G4">
         <v>19900701</v>
@@ -510,7 +516,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>19910630</v>
@@ -522,33 +528,562 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G5">
         <v>19910401</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>7</v>
+      <c r="A6">
+        <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>19990930</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>19990701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>20051231</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>20051001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>20100331</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>20100101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>20100630</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>20100401</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>20101231</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>20101001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C11">
+        <v>20140331</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>20140101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>20140630</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <v>20140401</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>20140930</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>20140701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>20141231</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <v>20141001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="C15">
+        <v>20150331</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>20150101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>20150630</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16">
+        <v>20150401</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>20151231</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17">
+        <v>20151001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>20160331</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18">
+        <v>20160101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>20160930</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19">
+        <v>20160701</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>20161231</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20">
+        <v>20161001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>20170331</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21">
+        <v>20170101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>20170630</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22">
+        <v>20170401</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>20170930</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23">
+        <v>20170701</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>20171231</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24">
+        <v>20171001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>20180331</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25">
+        <v>20180101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>20180630</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26">
+        <v>20180401</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
+      <c r="C27">
+        <v>20180930</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27">
+        <v>20180701</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
         <v>11</v>
+      </c>
+      <c r="C28">
+        <v>20180930</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28">
+        <v>20180701</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>20181231</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29">
+        <v>20181001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>